<commit_message>
Updated data - epochs are now longer, which changes the LI values very slightly
</commit_message>
<xml_diff>
--- a/filelist_L1_L2.xlsx
+++ b/filelist_L1_L2.xlsx
@@ -1,122 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23802"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_6604DB4CC928CEDC1A455E91F37DD9E2AB4B3522" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="L1" sheetId="1" r:id="rId1"/>
     <sheet name="L2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>trial1</t>
-  </si>
-  <si>
-    <t>trial2</t>
-  </si>
-  <si>
-    <t>trial3</t>
-  </si>
-  <si>
-    <t>trial4</t>
-  </si>
-  <si>
-    <t>trial5</t>
-  </si>
-  <si>
-    <t>trial6</t>
-  </si>
-  <si>
-    <t>trial7</t>
-  </si>
-  <si>
-    <t>trial8</t>
-  </si>
-  <si>
-    <t>trial9</t>
-  </si>
-  <si>
-    <t>trial10</t>
-  </si>
-  <si>
-    <t>trial11</t>
-  </si>
-  <si>
-    <t>trial12</t>
-  </si>
-  <si>
-    <t>trial13</t>
-  </si>
-  <si>
-    <t>trial14</t>
-  </si>
-  <si>
-    <t>trial15</t>
-  </si>
-  <si>
-    <t>trial16</t>
-  </si>
-  <si>
-    <t>trial17</t>
-  </si>
-  <si>
-    <t>trial18</t>
-  </si>
-  <si>
-    <t>trial19</t>
-  </si>
-  <si>
-    <t>trial20</t>
-  </si>
-  <si>
-    <t>trial21</t>
-  </si>
-  <si>
-    <t>trial22</t>
-  </si>
-  <si>
-    <t>trial23</t>
-  </si>
-  <si>
-    <t>trial11...11</t>
-  </si>
-  <si>
-    <t>trial11...12</t>
-  </si>
-  <si>
-    <t>trial21...21</t>
-  </si>
-  <si>
-    <t>trial21...22</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -165,14 +64,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -219,7 +110,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,27 +142,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -303,24 +176,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -496,88 +351,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>trial1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>trial2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>trial3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>trial4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>trial5</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>trial6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>trial7</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>trial8</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>trial9</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>trial10</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>trial11</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>trial12</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>trial13</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>trial14</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>trial15</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>trial16</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>trial17</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>trial18</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>trial19</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>trial20</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>trial21</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>trial22</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>trial23</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2">
         <v>14</v>
       </c>
@@ -651,7 +554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3">
       <c r="A3">
         <v>16</v>
       </c>
@@ -725,7 +628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4">
       <c r="A4">
         <v>17</v>
       </c>
@@ -799,7 +702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5">
       <c r="A5">
         <v>20</v>
       </c>
@@ -864,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="V5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W5">
         <v>1</v>
@@ -873,7 +776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6">
       <c r="A6">
         <v>22</v>
       </c>
@@ -947,7 +850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7">
       <c r="A7">
         <v>24</v>
       </c>
@@ -1021,7 +924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8">
       <c r="A8">
         <v>26</v>
       </c>
@@ -1095,7 +998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9">
       <c r="A9">
         <v>27</v>
       </c>
@@ -1169,7 +1072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10">
       <c r="A10">
         <v>28</v>
       </c>
@@ -1243,7 +1146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11">
       <c r="A11">
         <v>31</v>
       </c>
@@ -1317,7 +1220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12">
       <c r="A12">
         <v>32</v>
       </c>
@@ -1361,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="O12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="P12">
         <v>1</v>
@@ -1391,7 +1294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13">
       <c r="A13">
         <v>36</v>
       </c>
@@ -1465,7 +1368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14">
       <c r="A14">
         <v>37</v>
       </c>
@@ -1539,7 +1442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15">
       <c r="A15">
         <v>39</v>
       </c>
@@ -1613,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16">
       <c r="A16">
         <v>40</v>
       </c>
@@ -1687,7 +1590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17">
       <c r="A17">
         <v>41</v>
       </c>
@@ -1761,7 +1664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18">
       <c r="A18">
         <v>42</v>
       </c>
@@ -1835,7 +1738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19">
       <c r="A19">
         <v>43</v>
       </c>
@@ -1909,7 +1812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20">
       <c r="A20">
         <v>44</v>
       </c>
@@ -1983,7 +1886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21">
       <c r="A21">
         <v>45</v>
       </c>
@@ -2057,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22">
       <c r="A22">
         <v>46</v>
       </c>
@@ -2131,7 +2034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23">
       <c r="A23">
         <v>48</v>
       </c>
@@ -2205,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24">
       <c r="A24">
         <v>49</v>
       </c>
@@ -2279,7 +2182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25">
       <c r="A25">
         <v>51</v>
       </c>
@@ -2353,7 +2256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:24">
+    <row r="26">
       <c r="A26">
         <v>53</v>
       </c>
@@ -2427,7 +2330,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:24">
+    <row r="27">
       <c r="A27">
         <v>54</v>
       </c>
@@ -2507,88 +2410,136 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>trial1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>trial2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>trial3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>trial4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>trial5</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>trial6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>trial7</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>trial8</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>trial9</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>trial11...11</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>trial11...12</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>trial12</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>trial13</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>trial14</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>trial15</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>trial16</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>trial17</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>trial18</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>trial19</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>trial21...21</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>trial21...22</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>trial22</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>trial23</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2">
         <v>14</v>
       </c>
@@ -2596,7 +2547,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2662,7 +2613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3">
       <c r="A3">
         <v>16</v>
       </c>
@@ -2736,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4">
       <c r="A4">
         <v>17</v>
       </c>
@@ -2759,7 +2710,7 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -2810,7 +2761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5">
       <c r="A5">
         <v>20</v>
       </c>
@@ -2833,7 +2784,7 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -2884,7 +2835,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6">
       <c r="A6">
         <v>22</v>
       </c>
@@ -2958,7 +2909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7">
       <c r="A7">
         <v>24</v>
       </c>
@@ -2990,7 +2941,7 @@
         <v>1</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -3002,7 +2953,7 @@
         <v>1</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="P7">
         <v>1</v>
@@ -3032,7 +2983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8">
       <c r="A8">
         <v>26</v>
       </c>
@@ -3049,7 +3000,7 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -3106,7 +3057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9">
       <c r="A9">
         <v>27</v>
       </c>
@@ -3144,7 +3095,7 @@
         <v>1</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -3180,7 +3131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10">
       <c r="A10">
         <v>28</v>
       </c>
@@ -3239,7 +3190,7 @@
         <v>1</v>
       </c>
       <c r="T10">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="U10">
         <v>1</v>
@@ -3254,7 +3205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11">
       <c r="A11">
         <v>31</v>
       </c>
@@ -3328,7 +3279,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12">
       <c r="A12">
         <v>32</v>
       </c>
@@ -3402,7 +3353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13">
       <c r="A13">
         <v>36</v>
       </c>
@@ -3476,7 +3427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14">
       <c r="A14">
         <v>37</v>
       </c>
@@ -3550,7 +3501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15">
       <c r="A15">
         <v>39</v>
       </c>
@@ -3624,7 +3575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16">
       <c r="A16">
         <v>40</v>
       </c>
@@ -3650,7 +3601,7 @@
         <v>1</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -3698,7 +3649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17">
       <c r="A17">
         <v>41</v>
       </c>
@@ -3772,7 +3723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18">
       <c r="A18">
         <v>42</v>
       </c>
@@ -3846,7 +3797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19">
       <c r="A19">
         <v>43</v>
       </c>
@@ -3920,7 +3871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20">
       <c r="A20">
         <v>44</v>
       </c>
@@ -3976,7 +3927,7 @@
         <v>1</v>
       </c>
       <c r="S20">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="T20">
         <v>1</v>
@@ -3994,7 +3945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21">
       <c r="A21">
         <v>45</v>
       </c>
@@ -4056,7 +4007,7 @@
         <v>1</v>
       </c>
       <c r="U21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V21">
         <v>1</v>
@@ -4068,7 +4019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22">
       <c r="A22">
         <v>46</v>
       </c>
@@ -4142,12 +4093,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23">
       <c r="A23">
         <v>48</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -4216,12 +4167,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24">
       <c r="A24">
         <v>49</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -4290,7 +4241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25">
       <c r="A25">
         <v>51</v>
       </c>
@@ -4364,12 +4315,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:24">
+    <row r="26">
       <c r="A26">
         <v>53</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -4438,7 +4389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:24">
+    <row r="27">
       <c r="A27">
         <v>54</v>
       </c>

</xml_diff>